<commit_message>
add test cases and new .feature
</commit_message>
<xml_diff>
--- a/Plan de pruebas MielesSAS.xlsx
+++ b/Plan de pruebas MielesSAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Felipe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Felipe\Documents\Karate Automation\RetoQAAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E347556-DDA8-470E-8482-B2741A34C088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3902BE67-AB7A-4341-ACB2-094B2D5D87D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7011E6BA-1892-46C0-AB29-948751CC6DB9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7011E6BA-1892-46C0-AB29-948751CC6DB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Pruebas" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
   <si>
     <t>SISTEMA:</t>
   </si>
@@ -347,16 +347,34 @@
   <si>
     <t>Fallido</t>
   </si>
+  <si>
+    <t>Consulta de todos los usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el servicio https://reqres.in/api/unknown debera retornar una lista de clientes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuarios previamente creados </t>
+  </si>
+  <si>
+    <t>el servicio debera permitir consultar la totalidad de usuarios</t>
+  </si>
+  <si>
+    <t>enviar peticion de tipo get al servicio https://reqres.in/api/unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el servicio debera retornar con un http code = 200 y la informacion de los clientes como nombre apellido email id avatar dentro de un objeto llamado data </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="[$-80A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
-    <numFmt numFmtId="174" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-80A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -1377,8 +1395,8 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -1406,7 +1424,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1426,89 +1444,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1528,10 +1474,10 @@
     <xf numFmtId="0" fontId="23" fillId="26" borderId="0" xfId="65" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="23" fillId="26" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="23" fillId="26" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="174" fontId="23" fillId="26" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="23" fillId="26" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="26" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1557,7 +1503,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="30" fillId="26" borderId="24" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="30" fillId="26" borderId="24" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1568,26 +1514,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="26" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1595,26 +1521,6 @@
     <xf numFmtId="0" fontId="35" fillId="27" borderId="27" xfId="64" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="26" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1627,26 +1533,14 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="26" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="26" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="26" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1657,18 +1551,6 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="26" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
@@ -1682,6 +1564,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="72">
     <cellStyle name="_Capturas" xfId="2" xr:uid="{C50F674E-F102-4FD6-A16D-F69D6C67438C}"/>
@@ -2111,19 +2121,19 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" customHeight="1" thickBot="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="49"/>
     </row>
     <row r="6" spans="1:2" ht="228.75" customHeight="1" thickBot="1">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="51"/>
     </row>
     <row r="7" spans="1:2" ht="30.75" thickBot="1">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2131,17 +2141,17 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="54"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="55" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2149,55 +2159,55 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="18"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="56"/>
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="25" t="s">
+      <c r="A13" s="56"/>
+      <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="18"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="18"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="18"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="18"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A19" s="19"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="55" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2205,151 +2215,151 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="18"/>
+      <c r="A21" s="56"/>
       <c r="B21" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="18"/>
+      <c r="A22" s="56"/>
       <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A23" s="18"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="61"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="52"/>
     </row>
     <row r="26" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="11"/>
+      <c r="B26" s="54"/>
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="63"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="9"/>
     </row>
     <row r="29" spans="1:2" ht="15" customHeight="1">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="24"/>
+      <c r="B29" s="9"/>
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="26"/>
+      <c r="B30" s="59"/>
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="22"/>
+      <c r="B31" s="65"/>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B32" s="66"/>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="22"/>
+      <c r="B33" s="65"/>
     </row>
     <row r="34" spans="1:2" ht="15" customHeight="1">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="22"/>
+      <c r="B34" s="65"/>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="22"/>
+      <c r="B35" s="65"/>
     </row>
     <row r="36" spans="1:2" ht="15" customHeight="1">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="31"/>
+      <c r="B36" s="70"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="22"/>
+      <c r="B37" s="65"/>
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="31"/>
+      <c r="B38" s="70"/>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="22"/>
+      <c r="B39" s="65"/>
     </row>
     <row r="40" spans="1:2" ht="30" customHeight="1" thickBot="1">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="34"/>
+      <c r="B40" s="68"/>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8"/>
+      <c r="A41" s="60"/>
+      <c r="B41" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:A19"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2361,7 +2371,7 @@
   <dimension ref="A2:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2377,433 +2387,449 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="47"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="37"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="35"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="50">
+      <c r="B6" s="26">
         <v>45420</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="35"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="38"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="35"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" ht="33.75">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="30" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="42.75" customHeight="1">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="65">
+      <c r="E9" s="31">
         <v>1</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="G9" s="33" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="68"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="52">
+      <c r="A10" s="75"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="28">
         <v>2</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="69" t="s">
+      <c r="G10" s="34" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="42.75" customHeight="1">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="28">
         <v>1</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="69" t="s">
+      <c r="G11" s="34" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.5">
-      <c r="A12" s="68"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="52">
+      <c r="A12" s="75"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="28">
         <v>2</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="G12" s="34" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="42.75" customHeight="1">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="28">
         <v>1</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="69" t="s">
+      <c r="G13" s="34" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="42.75">
-      <c r="A14" s="68"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="52">
+      <c r="A14" s="75"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="28">
         <v>2</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="F14" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="69" t="s">
+      <c r="G14" s="34" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="57" customHeight="1">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E15" s="28">
         <v>1</v>
       </c>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="69" t="s">
+      <c r="G15" s="34" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="42.75">
-      <c r="A16" s="68"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="52">
+      <c r="A16" s="75"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="28">
         <v>2</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="69" t="s">
+      <c r="G16" s="34" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="42.75">
-      <c r="A17" s="71" t="s">
+      <c r="A17" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="52">
+      <c r="E17" s="28">
         <v>1</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="69" t="s">
+      <c r="G17" s="34" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="28">
         <v>1</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="69" t="s">
+      <c r="G18" s="34" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="76"/>
-      <c r="B19" s="77"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="73">
+      <c r="A19" s="81"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="36">
         <v>2</v>
       </c>
-      <c r="F19" s="74" t="s">
+      <c r="F19" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="75" t="s">
+      <c r="G19" s="38" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="60"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="45"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
+    <row r="20" spans="1:7" ht="33" customHeight="1">
+      <c r="A20" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="28">
+        <v>1</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="55.5" customHeight="1">
+      <c r="A21" s="81"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="36">
+        <v>2</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="45"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="45"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="45"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="45"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="45"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="45"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="45"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="45"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="45"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="45"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:D19"/>
+  <mergeCells count="24">
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
@@ -2816,6 +2842,14 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2836,82 +2870,82 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:4">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="81">
+      <c r="C2" s="41">
         <v>1</v>
       </c>
-      <c r="D2" s="82"/>
+      <c r="D2" s="42"/>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="2:4" ht="60">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="44"/>
     </row>
     <row r="5" spans="2:4" ht="45">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="84"/>
+      <c r="D5" s="44"/>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="30" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="83">
+      <c r="B7" s="43">
         <v>1</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="44" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="83">
+      <c r="B8" s="43">
         <v>2</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="84" t="s">
+      <c r="D8" s="44" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B9" s="85">
+      <c r="B9" s="45">
         <v>3</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="47" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>